<commit_message>
Changes to landing.jsp & landing.java, modifications to Command.java to make it more useful and efficient.
</commit_message>
<xml_diff>
--- a/SQL/StoredProcedures/CommandMatrix.xlsx
+++ b/SQL/StoredProcedures/CommandMatrix.xlsx
@@ -5,14 +5,18 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jarp/Dropbox/Personal/WARP Worldwide/WARP Source/SQL/StoredProcedures/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jarp/Dropbox/Personal/WARP Worldwide/WARP Source/JWeb/SQL/StoredProcedures/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="45380" windowHeight="17600" tabRatio="500"/>
+    <workbookView xWindow="55340" yWindow="11260" windowWidth="23700" windowHeight="17540" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Commands" sheetId="1" r:id="rId1"/>
+    <sheet name="AttributeNames" sheetId="3" r:id="rId2"/>
+    <sheet name="Web Pages" sheetId="4" r:id="rId3"/>
+    <sheet name="Java Resources" sheetId="5" r:id="rId4"/>
+    <sheet name="Error Codes" sheetId="2" r:id="rId5"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -27,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="74">
   <si>
     <t>Command</t>
   </si>
@@ -47,57 +51,6 @@
     <t>getUserAccountByID</t>
   </si>
   <si>
-    <t>registerUserAccount</t>
-  </si>
-  <si>
-    <t>RegisterUserAccount</t>
-  </si>
-  <si>
-    <t>Parm 1</t>
-  </si>
-  <si>
-    <t>Parm 2</t>
-  </si>
-  <si>
-    <t>Parm 3</t>
-  </si>
-  <si>
-    <t>Parm 4</t>
-  </si>
-  <si>
-    <t>Parm 5</t>
-  </si>
-  <si>
-    <t>Parm 6</t>
-  </si>
-  <si>
-    <t>Parm 7</t>
-  </si>
-  <si>
-    <t>Parm 8</t>
-  </si>
-  <si>
-    <t>Parm 9</t>
-  </si>
-  <si>
-    <t>Parm 10</t>
-  </si>
-  <si>
-    <t>Parm 11</t>
-  </si>
-  <si>
-    <t>Parm 12</t>
-  </si>
-  <si>
-    <t>Parm 13</t>
-  </si>
-  <si>
-    <t>Parm 14</t>
-  </si>
-  <si>
-    <t>Parm 15</t>
-  </si>
-  <si>
     <t>CommandText</t>
   </si>
   <si>
@@ -113,26 +66,200 @@
     <t>EmailAddress</t>
   </si>
   <si>
-    <t>PassphraseHash</t>
-  </si>
-  <si>
     <t>Input Sample</t>
   </si>
   <si>
     <t>Output Sample</t>
   </si>
   <si>
-    <t>{"ProcStatus": "SUCCESS", "ProcMessage": "", "UserAccountID": 7}</t>
-  </si>
-  <si>
-    <t>{"Command":"RegisterUserAccount","AuID":1,"IuID":1,"MemberName":"GracieWarp","EmailAddress":"grace.arp@warpww.com","PassphraseHash":"1000:6a4f1f63c6fa1dcdc34c2087f3a2db1f7cc796d9a875d57c:b9affce6cd72c7c662251635e8bb30a04ab18d9701b92a09"}</t>
+    <t>RegisterMember</t>
+  </si>
+  <si>
+    <t>registerMember</t>
+  </si>
+  <si>
+    <t>{"Command":"RegisterMember","AuID":1,"IuID":1,"MemberName":"GracieWarp","EmailAddress":"grace.arp@warpww.com","PassphraseHash":"1000:6a4f1f63c6fa1dcdc34c2087f3a2db1f7cc796d9a875d57c:b9affce6cd72c7c662251635e8bb30a04ab18d9701b92a09"}</t>
+  </si>
+  <si>
+    <t>Error Sample</t>
+  </si>
+  <si>
+    <t>{"MemberID": 43, "ProcStatus": "ERROR", "ProcMessage": "1062 (23000): Duplicate entry '2-GracieWarp' for key 'uniqueName'"}</t>
+  </si>
+  <si>
+    <t>{"MemberID": 44, "MemberName": "PeterWarp", "ProcStatus": "SUCCESS", "ProcMessage": "", "EmailAddress": "peter.parker@warpww.com"}</t>
+  </si>
+  <si>
+    <t>Terminus</t>
+  </si>
+  <si>
+    <t>XX</t>
+  </si>
+  <si>
+    <t>GeneratePasswordResetToken</t>
+  </si>
+  <si>
+    <t>GetMemberList</t>
+  </si>
+  <si>
+    <t>getMemberList</t>
+  </si>
+  <si>
+    <t>ValidateSignon</t>
+  </si>
+  <si>
+    <t>validateSignon</t>
+  </si>
+  <si>
+    <t>Error Code</t>
+  </si>
+  <si>
+    <t>Invalid Command</t>
+  </si>
+  <si>
+    <t>Member ID In Use</t>
+  </si>
+  <si>
+    <t>ErrorMessage</t>
+  </si>
+  <si>
+    <t>jsonResults</t>
+  </si>
+  <si>
+    <t>Element Name</t>
+  </si>
+  <si>
+    <t>Attribute Name</t>
+  </si>
+  <si>
+    <t>Parameter Name</t>
+  </si>
+  <si>
+    <t>JSON Name</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>SQL Name</t>
+  </si>
+  <si>
+    <t>CommandName</t>
+  </si>
+  <si>
+    <t>NewMemberName</t>
+  </si>
+  <si>
+    <t>MemberNameKey</t>
+  </si>
+  <si>
+    <t>MemberID</t>
+  </si>
+  <si>
+    <t>ProcStatus</t>
+  </si>
+  <si>
+    <t>MessageSource</t>
+  </si>
+  <si>
+    <t>MessageCode</t>
+  </si>
+  <si>
+    <t>"ErrorMe</t>
+  </si>
+  <si>
+    <t>about.jsp</t>
+  </si>
+  <si>
+    <t>botdetect.jsp</t>
+  </si>
+  <si>
+    <t>contact.jsp</t>
+  </si>
+  <si>
+    <t>home.jsp</t>
+  </si>
+  <si>
+    <t>landing.jsp</t>
+  </si>
+  <si>
+    <t>login.jsp</t>
+  </si>
+  <si>
+    <t>membermanagement.jsp</t>
+  </si>
+  <si>
+    <t>mission.jsp</t>
+  </si>
+  <si>
+    <t>passphrasereminder.jsp</t>
+  </si>
+  <si>
+    <t>petersons.jsp</t>
+  </si>
+  <si>
+    <t>register.jsp</t>
+  </si>
+  <si>
+    <t>registrationconfirmation.jsp</t>
+  </si>
+  <si>
+    <t>signin.jsp</t>
+  </si>
+  <si>
+    <t>solutions.jsp</t>
+  </si>
+  <si>
+    <t>testgrid.jsp</t>
+  </si>
+  <si>
+    <t>web.xml</t>
+  </si>
+  <si>
+    <t>WEB-INF</t>
+  </si>
+  <si>
+    <t>&lt;root&gt;</t>
+  </si>
+  <si>
+    <t>index.jsp</t>
+  </si>
+  <si>
+    <t>sidebarsample.html</t>
+  </si>
+  <si>
+    <t>old.private.pem.txt</t>
+  </si>
+  <si>
+    <t>old.public.pem.txt</t>
+  </si>
+  <si>
+    <t>test.html</t>
+  </si>
+  <si>
+    <t>TomcatVersion.jsp</t>
+  </si>
+  <si>
+    <t>Command.java</t>
+  </si>
+  <si>
+    <t>Library</t>
+  </si>
+  <si>
+    <t>Change To Command Results</t>
+  </si>
+  <si>
+    <t>ComandResults</t>
+  </si>
+  <si>
+    <t>Replaces  jsonResults</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -176,6 +303,19 @@
       <name val="Monaco"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Menlo"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -203,7 +343,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -214,7 +354,19 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -492,30 +644,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:V8"/>
+  <dimension ref="A3:G10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.83203125" style="2"/>
-    <col min="2" max="2" width="21" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.1640625" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="36.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="7.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="12" width="7.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="18" width="9" style="2" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="35.83203125" style="2" customWidth="1"/>
-    <col min="20" max="20" width="22.6640625" style="2" customWidth="1"/>
-    <col min="21" max="16384" width="10.83203125" style="2"/>
+    <col min="4" max="4" width="46" style="2" customWidth="1"/>
+    <col min="5" max="5" width="43.5" style="2" customWidth="1"/>
+    <col min="6" max="6" width="33.33203125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="10.83203125" style="6"/>
+    <col min="8" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="5" t="s">
         <v>0</v>
@@ -524,110 +671,489 @@
         <v>1</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="I3" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="J3" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="K3" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="L3" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="M3" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="N3" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="O3" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="P3" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q3" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="R3" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="S3" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="T3" s="5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C4" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B5" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="C5" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C6" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C7" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="V7" s="6"/>
-    </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="G7" s="7"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B8" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B9" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B10" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:G18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.33203125" customWidth="1"/>
+    <col min="7" max="7" width="12.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="B1" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
+        <v>72</v>
+      </c>
+      <c r="C7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>37</v>
+      </c>
+      <c r="E8" t="s">
+        <v>37</v>
+      </c>
+      <c r="F8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="G8" s="2" t="s">
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B13" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B14" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B16" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B17" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B18" t="s">
+        <v>44</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:B23"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="8.33203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>68</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:C8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="25.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B2" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="C2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B3" s="10"/>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B4" s="10"/>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B5" s="10"/>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B6" s="10"/>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B7" s="10"/>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B8" s="10"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="15.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:2" ht="19" x14ac:dyDescent="0.25">
+      <c r="B2" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="H8" s="2" t="s">
+    </row>
+    <row r="3" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
         <v>27</v>
       </c>
-      <c r="I8" s="2" t="s">
+    </row>
+    <row r="4" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
         <v>28</v>
       </c>
-      <c r="S8" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="T8" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="V8" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
2017.12.30 - BOD Push.
</commit_message>
<xml_diff>
--- a/SQL/StoredProcedures/CommandMatrix.xlsx
+++ b/SQL/StoredProcedures/CommandMatrix.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="83">
   <si>
     <t>Command</t>
   </si>
@@ -253,6 +253,33 @@
   </si>
   <si>
     <t>Replaces  jsonResults</t>
+  </si>
+  <si>
+    <t>Contact WARP</t>
+  </si>
+  <si>
+    <t>About WARP</t>
+  </si>
+  <si>
+    <t>WARP's Mission</t>
+  </si>
+  <si>
+    <t>WARP Products</t>
+  </si>
+  <si>
+    <t>Partner with WARP</t>
+  </si>
+  <si>
+    <t>Careers - Get WARPed!</t>
+  </si>
+  <si>
+    <t>Support</t>
+  </si>
+  <si>
+    <t>Login</t>
+  </si>
+  <si>
+    <t>Register</t>
   </si>
 </sst>
 </file>
@@ -750,10 +777,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:G18"/>
+  <dimension ref="B1:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -766,7 +793,7 @@
     <col min="7" max="7" width="12.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" ht="19" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:9" ht="19" x14ac:dyDescent="0.25">
       <c r="B1" s="5" t="s">
         <v>31</v>
       </c>
@@ -786,43 +813,58 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="I3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="I4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>30</v>
       </c>
       <c r="C5" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="I5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="I6" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>72</v>
       </c>
       <c r="C7" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="I7" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>37</v>
       </c>
@@ -832,43 +874,55 @@
       <c r="F8" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="I8" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="I9" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="I10" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="I11" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
         <v>43</v>
       </c>

</xml_diff>